<commit_message>
Update Dictionnaire de données
</commit_message>
<xml_diff>
--- a/Modelization/Dictionnaire de donnaee.xlsx
+++ b/Modelization/Dictionnaire de donnaee.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="10455" windowHeight="5385" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="10455" windowHeight="5385" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Remaqrues" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="146">
   <si>
     <t>Code</t>
   </si>
@@ -464,8 +464,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -754,7 +754,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -789,7 +788,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -965,14 +963,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="29.28515625" customWidth="1"/>
     <col min="2" max="2" width="60.28515625" bestFit="1" customWidth="1"/>
@@ -981,7 +979,7 @@
     <col min="6" max="6" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="17" t="s">
         <v>56</v>
       </c>
@@ -993,7 +991,7 @@
       </c>
       <c r="F1" s="18"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1011,7 +1009,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="5" t="s">
         <v>48</v>
       </c>
@@ -1029,7 +1027,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="5" t="s">
         <v>50</v>
       </c>
@@ -1047,7 +1045,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="5" t="s">
         <v>52</v>
       </c>
@@ -1065,7 +1063,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="5" t="s">
         <v>53</v>
       </c>
@@ -1083,7 +1081,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
@@ -1101,7 +1099,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
@@ -1119,7 +1117,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
@@ -1137,7 +1135,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="7" t="s">
         <v>12</v>
       </c>
@@ -1155,7 +1153,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="7" t="s">
         <v>14</v>
       </c>
@@ -1173,7 +1171,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
@@ -1191,7 +1189,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="7" t="s">
         <v>18</v>
       </c>
@@ -1209,7 +1207,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="9" t="s">
         <v>26</v>
       </c>
@@ -1227,7 +1225,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="9" t="s">
         <v>28</v>
       </c>
@@ -1245,7 +1243,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="9" t="s">
         <v>21</v>
       </c>
@@ -1263,7 +1261,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="9" t="s">
         <v>24</v>
       </c>
@@ -1281,7 +1279,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="10" t="s">
         <v>30</v>
       </c>
@@ -1299,7 +1297,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="10" t="s">
         <v>33</v>
       </c>
@@ -1317,7 +1315,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="10" t="s">
         <v>35</v>
       </c>
@@ -1335,7 +1333,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="10" t="s">
         <v>37</v>
       </c>
@@ -1353,7 +1351,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="11" t="s">
         <v>39</v>
       </c>
@@ -1371,7 +1369,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="11" t="s">
         <v>41</v>
       </c>
@@ -1389,7 +1387,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="11" t="s">
         <v>43</v>
       </c>
@@ -1407,7 +1405,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="11" t="s">
         <v>45</v>
       </c>
@@ -1425,7 +1423,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="11" t="s">
         <v>24</v>
       </c>
@@ -1443,7 +1441,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="12" t="s">
         <v>80</v>
       </c>
@@ -1461,7 +1459,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>108</v>
       </c>
@@ -1469,7 +1467,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>110</v>
       </c>
@@ -1477,7 +1475,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>111</v>
       </c>
@@ -1485,7 +1483,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>113</v>
       </c>
@@ -1493,7 +1491,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>115</v>
       </c>
@@ -1501,7 +1499,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>117</v>
       </c>
@@ -1509,7 +1507,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>118</v>
       </c>
@@ -1517,7 +1515,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>120</v>
       </c>
@@ -1537,19 +1535,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>122</v>
       </c>
@@ -1557,7 +1555,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -1565,7 +1563,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -1573,7 +1571,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>126</v>
       </c>
@@ -1581,20 +1579,12 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>61</v>
       </c>
       <c r="B5" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>141</v>
-      </c>
-      <c r="B6" t="s">
-        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1603,20 +1593,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32.140625" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>66</v>
       </c>
@@ -1624,7 +1614,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>128</v>
       </c>
@@ -1632,7 +1622,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1640,7 +1630,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>131</v>
       </c>
@@ -1654,20 +1644,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31.28515625" customWidth="1"/>
     <col min="2" max="2" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>133</v>
       </c>
@@ -1675,7 +1665,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>135</v>
       </c>
@@ -1689,19 +1679,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>137</v>
       </c>
@@ -1715,16 +1705,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>122</v>
       </c>
@@ -1732,7 +1722,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>139</v>
       </c>
@@ -1746,16 +1736,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>140</v>
       </c>
@@ -1763,7 +1753,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>141</v>
       </c>
@@ -1771,7 +1761,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -1785,16 +1775,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>144</v>
       </c>

</xml_diff>

<commit_message>
Fix - Title of Entity in Menu not Work
</commit_message>
<xml_diff>
--- a/Modelization/Dictionnaire de donnaee.xlsx
+++ b/Modelization/Dictionnaire de donnaee.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ES-SARRAJ Fouad\Documents\GitHub\shop-management-solution\Modelization\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="10455" windowHeight="5385" activeTab="7"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="10455" windowHeight="5385" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Remaqrues" sheetId="1" r:id="rId1"/>
-    <sheet name="User" sheetId="2" r:id="rId2"/>
+    <sheet name="User-Utilisateur" sheetId="2" r:id="rId2"/>
     <sheet name="Article" sheetId="3" r:id="rId3"/>
     <sheet name="Order" sheetId="4" r:id="rId4"/>
-    <sheet name="Delivery" sheetId="5" r:id="rId5"/>
-    <sheet name="CategorieArticle" sheetId="6" r:id="rId6"/>
-    <sheet name="Provider" sheetId="7" r:id="rId7"/>
-    <sheet name="OrderLine" sheetId="8" r:id="rId8"/>
+    <sheet name="Delivery-Laivraison" sheetId="5" r:id="rId5"/>
+    <sheet name="CategorieArticle-CatégorieArtic" sheetId="6" r:id="rId6"/>
+    <sheet name="Provider-Fournisseur" sheetId="7" r:id="rId7"/>
+    <sheet name="OrderLine-LigneCommande" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -464,8 +469,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -675,6 +680,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -722,7 +730,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -754,9 +762,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -788,6 +797,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -963,14 +973,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.28515625" customWidth="1"/>
     <col min="2" max="2" width="60.28515625" bestFit="1" customWidth="1"/>
@@ -979,7 +989,7 @@
     <col min="6" max="6" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>56</v>
       </c>
@@ -991,7 +1001,7 @@
       </c>
       <c r="F1" s="18"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1009,7 +1019,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>48</v>
       </c>
@@ -1027,7 +1037,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>50</v>
       </c>
@@ -1045,7 +1055,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>52</v>
       </c>
@@ -1063,7 +1073,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>53</v>
       </c>
@@ -1081,7 +1091,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
@@ -1099,7 +1109,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
@@ -1117,7 +1127,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
@@ -1135,7 +1145,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>12</v>
       </c>
@@ -1153,7 +1163,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>14</v>
       </c>
@@ -1171,7 +1181,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
@@ -1189,7 +1199,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>18</v>
       </c>
@@ -1207,7 +1217,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>26</v>
       </c>
@@ -1225,7 +1235,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>28</v>
       </c>
@@ -1243,7 +1253,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>21</v>
       </c>
@@ -1261,7 +1271,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>24</v>
       </c>
@@ -1279,7 +1289,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>30</v>
       </c>
@@ -1297,7 +1307,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>33</v>
       </c>
@@ -1315,7 +1325,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>35</v>
       </c>
@@ -1333,7 +1343,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>37</v>
       </c>
@@ -1351,7 +1361,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>39</v>
       </c>
@@ -1369,7 +1379,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>41</v>
       </c>
@@ -1387,7 +1397,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>43</v>
       </c>
@@ -1405,7 +1415,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>45</v>
       </c>
@@ -1423,7 +1433,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>24</v>
       </c>
@@ -1441,7 +1451,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>80</v>
       </c>
@@ -1459,7 +1469,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>108</v>
       </c>
@@ -1467,7 +1477,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>110</v>
       </c>
@@ -1475,7 +1485,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>111</v>
       </c>
@@ -1483,7 +1493,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>113</v>
       </c>
@@ -1491,7 +1501,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>115</v>
       </c>
@@ -1499,7 +1509,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>117</v>
       </c>
@@ -1507,7 +1517,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>118</v>
       </c>
@@ -1515,7 +1525,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>120</v>
       </c>
@@ -1535,19 +1545,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>122</v>
       </c>
@@ -1555,7 +1565,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -1563,7 +1573,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -1571,7 +1581,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>126</v>
       </c>
@@ -1579,7 +1589,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>61</v>
       </c>
@@ -1593,20 +1603,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.140625" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>66</v>
       </c>
@@ -1614,7 +1624,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>128</v>
       </c>
@@ -1622,7 +1632,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1630,7 +1640,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>131</v>
       </c>
@@ -1644,20 +1654,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.28515625" customWidth="1"/>
     <col min="2" max="2" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>133</v>
       </c>
@@ -1665,7 +1675,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>135</v>
       </c>
@@ -1679,19 +1689,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>137</v>
       </c>
@@ -1705,16 +1715,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>122</v>
       </c>
@@ -1722,7 +1732,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>139</v>
       </c>
@@ -1736,16 +1746,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>140</v>
       </c>
@@ -1753,7 +1763,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>141</v>
       </c>
@@ -1761,7 +1771,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -1775,16 +1785,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>144</v>
       </c>

</xml_diff>